<commit_message>
add common I2C write funck in i2c_interface. start to write class for ina219, for Lora. Start to write UFO_Utils. Start to write UFO_Error (now only defs) Add socket task; Add code for tank control. Add lora pinout(docks), Lora DS, INA DS. Correct sockStructDefs
</commit_message>
<xml_diff>
--- a/docks/UFO_Pinout.xlsx
+++ b/docks/UFO_Pinout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\esppres_my_workspace\UFO_1\docks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21003CA9-F6E0-403D-9CA2-0F63D2F2D1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48936C9F-3200-47DE-852A-816AC684DBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="110">
   <si>
     <t>EN</t>
   </si>
@@ -336,6 +336,21 @@
   </si>
   <si>
     <t>UART3</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>M0</t>
+  </si>
+  <si>
+    <t>AUX</t>
+  </si>
+  <si>
+    <t>LORA</t>
+  </si>
+  <si>
+    <t>UART LORA</t>
   </si>
 </sst>
 </file>
@@ -456,7 +471,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="28">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -619,6 +634,24 @@
         <bgColor theme="0" tint="-0.249977111117893"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="57">
     <border>
@@ -1320,7 +1353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1565,38 +1598,239 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1616,12 +1850,6 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1659,9 +1887,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1682,60 +1907,6 @@
     <xf numFmtId="0" fontId="10" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1763,169 +1934,61 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2209,8 +2272,8 @@
   <sheetPr codeName="Лист9"/>
   <dimension ref="B1:AJ33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AD12" sqref="AD12:AJ13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AG33" sqref="AG33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2234,165 +2297,165 @@
   <sheetData>
     <row r="1" spans="2:36" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:36" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="175" t="s">
+      <c r="B2" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="177"/>
-      <c r="I2" s="184" t="s">
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="107" t="s">
         <v>85</v>
       </c>
-      <c r="J2" s="185"/>
-      <c r="K2" s="132" t="s">
+      <c r="J2" s="108"/>
+      <c r="K2" s="136" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="153" t="s">
+      <c r="L2" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="130" t="s">
+      <c r="M2" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="167" t="s">
+      <c r="N2" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="163" t="s">
+      <c r="O2" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="161" t="s">
+      <c r="P2" s="126" t="s">
         <v>86</v>
       </c>
-      <c r="Q2" s="155" t="s">
+      <c r="Q2" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="151" t="s">
+      <c r="R2" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="165" t="s">
+      <c r="S2" s="130" t="s">
         <v>92</v>
       </c>
-      <c r="T2" s="169" t="s">
+      <c r="T2" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="171" t="s">
+      <c r="U2" s="134" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="161" t="s">
+      <c r="V2" s="126" t="s">
         <v>86</v>
       </c>
-      <c r="W2" s="163" t="s">
+      <c r="W2" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="X2" s="167" t="s">
+      <c r="X2" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" s="130" t="s">
+      <c r="Y2" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="Z2" s="153" t="s">
+      <c r="Z2" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="AA2" s="132" t="s">
+      <c r="AA2" s="136" t="s">
         <v>18</v>
       </c>
-      <c r="AB2" s="188" t="s">
+      <c r="AB2" s="111" t="s">
         <v>85</v>
       </c>
-      <c r="AC2" s="184"/>
-      <c r="AD2" s="175" t="s">
+      <c r="AC2" s="107"/>
+      <c r="AD2" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="AE2" s="176"/>
-      <c r="AF2" s="176"/>
-      <c r="AG2" s="176"/>
-      <c r="AH2" s="176"/>
-      <c r="AI2" s="176"/>
-      <c r="AJ2" s="177"/>
+      <c r="AE2" s="99"/>
+      <c r="AF2" s="99"/>
+      <c r="AG2" s="99"/>
+      <c r="AH2" s="99"/>
+      <c r="AI2" s="99"/>
+      <c r="AJ2" s="100"/>
     </row>
     <row r="3" spans="2:36" s="2" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="178"/>
-      <c r="C3" s="179"/>
-      <c r="D3" s="179"/>
-      <c r="E3" s="179"/>
-      <c r="F3" s="179"/>
-      <c r="G3" s="179"/>
-      <c r="H3" s="180"/>
-      <c r="I3" s="186"/>
-      <c r="J3" s="187"/>
-      <c r="K3" s="133"/>
-      <c r="L3" s="154"/>
-      <c r="M3" s="131"/>
-      <c r="N3" s="168"/>
-      <c r="O3" s="164"/>
-      <c r="P3" s="162"/>
-      <c r="Q3" s="156"/>
-      <c r="R3" s="152"/>
-      <c r="S3" s="166"/>
-      <c r="T3" s="170"/>
-      <c r="U3" s="172"/>
-      <c r="V3" s="162"/>
-      <c r="W3" s="164"/>
-      <c r="X3" s="168"/>
-      <c r="Y3" s="131"/>
-      <c r="Z3" s="154"/>
-      <c r="AA3" s="133"/>
-      <c r="AB3" s="189"/>
-      <c r="AC3" s="186"/>
-      <c r="AD3" s="178"/>
-      <c r="AE3" s="179"/>
-      <c r="AF3" s="179"/>
-      <c r="AG3" s="179"/>
-      <c r="AH3" s="179"/>
-      <c r="AI3" s="179"/>
-      <c r="AJ3" s="180"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="110"/>
+      <c r="K3" s="137"/>
+      <c r="L3" s="123"/>
+      <c r="M3" s="129"/>
+      <c r="N3" s="114"/>
+      <c r="O3" s="116"/>
+      <c r="P3" s="127"/>
+      <c r="Q3" s="125"/>
+      <c r="R3" s="121"/>
+      <c r="S3" s="131"/>
+      <c r="T3" s="133"/>
+      <c r="U3" s="135"/>
+      <c r="V3" s="127"/>
+      <c r="W3" s="116"/>
+      <c r="X3" s="114"/>
+      <c r="Y3" s="129"/>
+      <c r="Z3" s="123"/>
+      <c r="AA3" s="137"/>
+      <c r="AB3" s="112"/>
+      <c r="AC3" s="109"/>
+      <c r="AD3" s="101"/>
+      <c r="AE3" s="102"/>
+      <c r="AF3" s="102"/>
+      <c r="AG3" s="102"/>
+      <c r="AH3" s="102"/>
+      <c r="AI3" s="102"/>
+      <c r="AJ3" s="103"/>
     </row>
     <row r="4" spans="2:36" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H4" s="134"/>
-      <c r="I4" s="134"/>
-      <c r="J4" s="134"/>
-      <c r="K4" s="134"/>
-      <c r="L4" s="134"/>
-      <c r="M4" s="134"/>
-      <c r="N4" s="134"/>
-      <c r="O4" s="134"/>
-      <c r="P4" s="134"/>
-      <c r="Q4" s="134"/>
-      <c r="R4" s="134"/>
-      <c r="S4" s="134"/>
-      <c r="T4" s="134"/>
-      <c r="U4" s="134"/>
-      <c r="V4" s="134"/>
-      <c r="W4" s="134"/>
-      <c r="X4" s="134"/>
-      <c r="Y4" s="134"/>
-      <c r="Z4" s="134"/>
-      <c r="AA4" s="134"/>
-      <c r="AB4" s="134"/>
-      <c r="AC4" s="134"/>
-      <c r="AD4" s="134"/>
+      <c r="H4" s="138"/>
+      <c r="I4" s="138"/>
+      <c r="J4" s="138"/>
+      <c r="K4" s="138"/>
+      <c r="L4" s="138"/>
+      <c r="M4" s="138"/>
+      <c r="N4" s="138"/>
+      <c r="O4" s="138"/>
+      <c r="P4" s="138"/>
+      <c r="Q4" s="138"/>
+      <c r="R4" s="138"/>
+      <c r="S4" s="138"/>
+      <c r="T4" s="138"/>
+      <c r="U4" s="138"/>
+      <c r="V4" s="138"/>
+      <c r="W4" s="138"/>
+      <c r="X4" s="138"/>
+      <c r="Y4" s="138"/>
+      <c r="Z4" s="138"/>
+      <c r="AA4" s="138"/>
+      <c r="AB4" s="138"/>
+      <c r="AC4" s="138"/>
+      <c r="AD4" s="138"/>
     </row>
     <row r="5" spans="2:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="181" t="s">
+      <c r="B5" s="104" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="182"/>
-      <c r="D5" s="182"/>
-      <c r="E5" s="182"/>
-      <c r="F5" s="182"/>
-      <c r="G5" s="182"/>
-      <c r="H5" s="183"/>
-      <c r="AD5" s="181" t="s">
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="106"/>
+      <c r="AD5" s="104" t="s">
         <v>87</v>
       </c>
-      <c r="AE5" s="182"/>
-      <c r="AF5" s="182"/>
-      <c r="AG5" s="182"/>
-      <c r="AH5" s="182"/>
-      <c r="AI5" s="182"/>
-      <c r="AJ5" s="183"/>
+      <c r="AE5" s="105"/>
+      <c r="AF5" s="105"/>
+      <c r="AG5" s="105"/>
+      <c r="AH5" s="105"/>
+      <c r="AI5" s="105"/>
+      <c r="AJ5" s="106"/>
     </row>
     <row r="6" spans="2:36" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="50">
@@ -2416,17 +2479,17 @@
       <c r="H6" s="52">
         <v>0</v>
       </c>
-      <c r="AD6" s="50">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="51">
-        <v>1</v>
-      </c>
-      <c r="AF6" s="51">
-        <v>2</v>
-      </c>
-      <c r="AG6" s="51">
-        <v>3</v>
+      <c r="AD6" s="203" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE6" s="205" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF6" s="207" t="s">
+        <v>99</v>
+      </c>
+      <c r="AG6" s="210" t="s">
+        <v>108</v>
       </c>
       <c r="AH6" s="51">
         <v>4</v>
@@ -2439,17 +2502,17 @@
       </c>
     </row>
     <row r="7" spans="2:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="190"/>
-      <c r="C7" s="191"/>
-      <c r="D7" s="191"/>
-      <c r="E7" s="191"/>
-      <c r="F7" s="191"/>
-      <c r="G7" s="191"/>
-      <c r="H7" s="192"/>
-      <c r="I7" s="159" t="s">
+      <c r="B7" s="94"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="146" t="s">
         <v>84</v>
       </c>
-      <c r="J7" s="160"/>
+      <c r="J7" s="147"/>
       <c r="K7" s="53" t="s">
         <v>20</v>
       </c>
@@ -2499,10 +2562,10 @@
       <c r="AA7" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="AB7" s="84" t="s">
+      <c r="AB7" s="194" t="s">
         <v>94</v>
       </c>
-      <c r="AC7" s="85"/>
+      <c r="AC7" s="195"/>
       <c r="AD7" s="60"/>
       <c r="AE7" s="42"/>
       <c r="AF7" s="42"/>
@@ -2519,8 +2582,8 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="29"/>
-      <c r="I8" s="193"/>
-      <c r="J8" s="194"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="97"/>
       <c r="K8" s="8" t="s">
         <v>23</v>
       </c>
@@ -2570,17 +2633,17 @@
       <c r="AA8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AB8" s="82" t="s">
+      <c r="AB8" s="148" t="s">
         <v>6</v>
       </c>
-      <c r="AC8" s="83"/>
-      <c r="AD8" s="28" t="s">
+      <c r="AC8" s="84"/>
+      <c r="AD8" s="204" t="s">
         <v>97</v>
       </c>
-      <c r="AE8" s="15" t="s">
+      <c r="AE8" s="206" t="s">
         <v>98</v>
       </c>
-      <c r="AF8" s="15" t="s">
+      <c r="AF8" s="208" t="s">
         <v>99</v>
       </c>
       <c r="AG8" s="15"/>
@@ -2596,8 +2659,8 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="29"/>
-      <c r="I9" s="193"/>
-      <c r="J9" s="194"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="97"/>
       <c r="K9" s="8" t="s">
         <v>23</v>
       </c>
@@ -2647,19 +2710,19 @@
       <c r="AA9" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="AB9" s="173" t="s">
+      <c r="AB9" s="149" t="s">
         <v>76</v>
       </c>
-      <c r="AC9" s="174"/>
-      <c r="AD9" s="195" t="s">
+      <c r="AC9" s="150"/>
+      <c r="AD9" s="88" t="s">
         <v>101</v>
       </c>
-      <c r="AE9" s="114"/>
-      <c r="AF9" s="114"/>
-      <c r="AG9" s="114"/>
-      <c r="AH9" s="114"/>
-      <c r="AI9" s="114"/>
-      <c r="AJ9" s="196"/>
+      <c r="AE9" s="89"/>
+      <c r="AF9" s="89"/>
+      <c r="AG9" s="89"/>
+      <c r="AH9" s="89"/>
+      <c r="AI9" s="89"/>
+      <c r="AJ9" s="90"/>
     </row>
     <row r="10" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B10" s="28"/>
@@ -2669,8 +2732,8 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="29"/>
-      <c r="I10" s="193"/>
-      <c r="J10" s="194"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="97"/>
       <c r="K10" s="8" t="s">
         <v>23</v>
       </c>
@@ -2720,17 +2783,17 @@
       <c r="AA10" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="AB10" s="173" t="s">
+      <c r="AB10" s="149" t="s">
         <v>77</v>
       </c>
-      <c r="AC10" s="174"/>
-      <c r="AD10" s="197"/>
-      <c r="AE10" s="198"/>
-      <c r="AF10" s="198"/>
-      <c r="AG10" s="198"/>
-      <c r="AH10" s="198"/>
-      <c r="AI10" s="198"/>
-      <c r="AJ10" s="199"/>
+      <c r="AC10" s="150"/>
+      <c r="AD10" s="91"/>
+      <c r="AE10" s="92"/>
+      <c r="AF10" s="92"/>
+      <c r="AG10" s="92"/>
+      <c r="AH10" s="92"/>
+      <c r="AI10" s="92"/>
+      <c r="AJ10" s="93"/>
     </row>
     <row r="11" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B11" s="28"/>
@@ -2740,8 +2803,8 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="29"/>
-      <c r="I11" s="193"/>
-      <c r="J11" s="194"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="97"/>
       <c r="K11" s="8" t="s">
         <v>23</v>
       </c>
@@ -2791,17 +2854,17 @@
       <c r="AA11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AB11" s="82" t="s">
+      <c r="AB11" s="148" t="s">
         <v>5</v>
       </c>
-      <c r="AC11" s="83"/>
-      <c r="AD11" s="28" t="s">
+      <c r="AC11" s="84"/>
+      <c r="AD11" s="204" t="s">
         <v>97</v>
       </c>
-      <c r="AE11" s="15" t="s">
+      <c r="AE11" s="206" t="s">
         <v>98</v>
       </c>
-      <c r="AF11" s="15" t="s">
+      <c r="AF11" s="208" t="s">
         <v>99</v>
       </c>
       <c r="AG11" s="15"/>
@@ -2810,17 +2873,17 @@
       <c r="AJ11" s="29"/>
     </row>
     <row r="12" spans="2:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="201" t="s">
+      <c r="B12" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="C12" s="157"/>
-      <c r="D12" s="157"/>
-      <c r="E12" s="157"/>
-      <c r="F12" s="157"/>
-      <c r="G12" s="157"/>
-      <c r="H12" s="202"/>
-      <c r="I12" s="193"/>
-      <c r="J12" s="194"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="83"/>
+      <c r="J12" s="97"/>
       <c r="K12" s="8" t="s">
         <v>23</v>
       </c>
@@ -2870,32 +2933,32 @@
       <c r="AA12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AB12" s="82" t="s">
+      <c r="AB12" s="148" t="s">
         <v>95</v>
       </c>
-      <c r="AC12" s="83"/>
-      <c r="AD12" s="195" t="s">
+      <c r="AC12" s="84"/>
+      <c r="AD12" s="88" t="s">
         <v>104</v>
       </c>
-      <c r="AE12" s="114"/>
-      <c r="AF12" s="114"/>
-      <c r="AG12" s="114"/>
-      <c r="AH12" s="114"/>
-      <c r="AI12" s="114"/>
-      <c r="AJ12" s="196"/>
+      <c r="AE12" s="89"/>
+      <c r="AF12" s="89"/>
+      <c r="AG12" s="89"/>
+      <c r="AH12" s="89"/>
+      <c r="AI12" s="89"/>
+      <c r="AJ12" s="90"/>
     </row>
     <row r="13" spans="2:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="201" t="s">
+      <c r="B13" s="85" t="s">
         <v>103</v>
       </c>
-      <c r="C13" s="157"/>
-      <c r="D13" s="157"/>
-      <c r="E13" s="157"/>
-      <c r="F13" s="157"/>
-      <c r="G13" s="157"/>
-      <c r="H13" s="202"/>
-      <c r="I13" s="193"/>
-      <c r="J13" s="194"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="97"/>
       <c r="K13" s="8" t="s">
         <v>23</v>
       </c>
@@ -2945,17 +3008,17 @@
       <c r="AA13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AB13" s="82" t="s">
+      <c r="AB13" s="148" t="s">
         <v>96</v>
       </c>
-      <c r="AC13" s="83"/>
-      <c r="AD13" s="197"/>
-      <c r="AE13" s="198"/>
-      <c r="AF13" s="198"/>
-      <c r="AG13" s="198"/>
-      <c r="AH13" s="198"/>
-      <c r="AI13" s="198"/>
-      <c r="AJ13" s="199"/>
+      <c r="AC13" s="84"/>
+      <c r="AD13" s="91"/>
+      <c r="AE13" s="92"/>
+      <c r="AF13" s="92"/>
+      <c r="AG13" s="92"/>
+      <c r="AH13" s="92"/>
+      <c r="AI13" s="92"/>
+      <c r="AJ13" s="93"/>
     </row>
     <row r="14" spans="2:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="28"/>
@@ -2965,10 +3028,10 @@
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
       <c r="H14" s="29"/>
-      <c r="I14" s="157" t="s">
+      <c r="I14" s="86" t="s">
         <v>82</v>
       </c>
-      <c r="J14" s="158"/>
+      <c r="J14" s="145"/>
       <c r="K14" s="8" t="s">
         <v>23</v>
       </c>
@@ -3018,32 +3081,34 @@
       <c r="AA14" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="AB14" s="82" t="s">
+      <c r="AB14" s="148" t="s">
         <v>36</v>
       </c>
-      <c r="AC14" s="83"/>
+      <c r="AC14" s="84"/>
       <c r="AD14" s="28"/>
       <c r="AE14" s="15"/>
       <c r="AF14" s="15"/>
-      <c r="AG14" s="15"/>
+      <c r="AG14" s="209" t="s">
+        <v>105</v>
+      </c>
       <c r="AH14" s="15"/>
       <c r="AI14" s="15"/>
       <c r="AJ14" s="29"/>
     </row>
     <row r="15" spans="2:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="200" t="s">
+      <c r="B15" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="193"/>
-      <c r="D15" s="193"/>
-      <c r="E15" s="193"/>
-      <c r="F15" s="193"/>
-      <c r="G15" s="193"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="157" t="s">
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="83"/>
+      <c r="H15" s="84"/>
+      <c r="I15" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="J15" s="158"/>
+      <c r="J15" s="145"/>
       <c r="K15" s="8" t="s">
         <v>23</v>
       </c>
@@ -3093,32 +3158,36 @@
       <c r="AA15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AB15" s="82" t="s">
+      <c r="AB15" s="148" t="s">
         <v>7</v>
       </c>
-      <c r="AC15" s="83"/>
-      <c r="AD15" s="195" t="s">
+      <c r="AC15" s="84"/>
+      <c r="AD15" s="88" t="s">
         <v>100</v>
       </c>
-      <c r="AE15" s="114"/>
-      <c r="AF15" s="114"/>
-      <c r="AG15" s="114"/>
-      <c r="AH15" s="114"/>
-      <c r="AI15" s="114"/>
-      <c r="AJ15" s="196"/>
+      <c r="AE15" s="89"/>
+      <c r="AF15" s="89"/>
+      <c r="AG15" s="211" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH15" s="88" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI15" s="89"/>
+      <c r="AJ15" s="89"/>
     </row>
     <row r="16" spans="2:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="200" t="s">
+      <c r="B16" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="193"/>
-      <c r="D16" s="193"/>
-      <c r="E16" s="193"/>
-      <c r="F16" s="193"/>
-      <c r="G16" s="193"/>
-      <c r="H16" s="83"/>
-      <c r="I16" s="193"/>
-      <c r="J16" s="194"/>
+      <c r="C16" s="83"/>
+      <c r="D16" s="83"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="83"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="83"/>
+      <c r="J16" s="97"/>
       <c r="K16" s="8" t="s">
         <v>23</v>
       </c>
@@ -3168,28 +3237,28 @@
       <c r="AA16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AB16" s="82" t="s">
+      <c r="AB16" s="148" t="s">
         <v>8</v>
       </c>
-      <c r="AC16" s="83"/>
-      <c r="AD16" s="197"/>
-      <c r="AE16" s="198"/>
-      <c r="AF16" s="198"/>
-      <c r="AG16" s="198"/>
-      <c r="AH16" s="198"/>
-      <c r="AI16" s="198"/>
-      <c r="AJ16" s="199"/>
+      <c r="AC16" s="84"/>
+      <c r="AD16" s="91"/>
+      <c r="AE16" s="92"/>
+      <c r="AF16" s="92"/>
+      <c r="AG16" s="212"/>
+      <c r="AH16" s="91"/>
+      <c r="AI16" s="92"/>
+      <c r="AJ16" s="92"/>
     </row>
     <row r="17" spans="2:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="200" t="s">
+      <c r="B17" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="193"/>
-      <c r="D17" s="193"/>
-      <c r="E17" s="193"/>
-      <c r="F17" s="193"/>
-      <c r="G17" s="193"/>
-      <c r="H17" s="83"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="83"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="83"/>
+      <c r="H17" s="84"/>
       <c r="I17" s="38" t="s">
         <v>78</v>
       </c>
@@ -3245,12 +3314,14 @@
       <c r="AA17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AB17" s="82"/>
-      <c r="AC17" s="83"/>
+      <c r="AB17" s="148"/>
+      <c r="AC17" s="84"/>
       <c r="AD17" s="28"/>
       <c r="AE17" s="15"/>
       <c r="AF17" s="15"/>
-      <c r="AG17" s="15"/>
+      <c r="AG17" s="209" t="s">
+        <v>107</v>
+      </c>
       <c r="AH17" s="15"/>
       <c r="AI17" s="15"/>
       <c r="AJ17" s="29"/>
@@ -3318,28 +3389,30 @@
       <c r="AA18" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="AB18" s="82" t="s">
+      <c r="AB18" s="148" t="s">
         <v>90</v>
       </c>
-      <c r="AC18" s="83"/>
+      <c r="AC18" s="84"/>
       <c r="AD18" s="28"/>
       <c r="AE18" s="15"/>
       <c r="AF18" s="15"/>
-      <c r="AG18" s="15"/>
+      <c r="AG18" s="209" t="s">
+        <v>106</v>
+      </c>
       <c r="AH18" s="15"/>
       <c r="AI18" s="15"/>
       <c r="AJ18" s="29"/>
     </row>
     <row r="19" spans="2:36" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="200" t="s">
+      <c r="B19" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="193"/>
-      <c r="D19" s="193"/>
-      <c r="E19" s="193"/>
-      <c r="F19" s="193"/>
-      <c r="G19" s="193"/>
-      <c r="H19" s="83"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="83"/>
+      <c r="F19" s="83"/>
+      <c r="G19" s="83"/>
+      <c r="H19" s="84"/>
       <c r="I19" s="38" t="s">
         <v>80</v>
       </c>
@@ -3417,16 +3490,16 @@
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="29"/>
-      <c r="I20" s="86" t="s">
+      <c r="I20" s="196" t="s">
         <v>2</v>
       </c>
-      <c r="J20" s="86"/>
-      <c r="K20" s="86"/>
-      <c r="L20" s="86"/>
-      <c r="M20" s="86"/>
-      <c r="N20" s="86"/>
-      <c r="O20" s="86"/>
-      <c r="P20" s="86"/>
+      <c r="J20" s="196"/>
+      <c r="K20" s="196"/>
+      <c r="L20" s="196"/>
+      <c r="M20" s="196"/>
+      <c r="N20" s="196"/>
+      <c r="O20" s="196"/>
+      <c r="P20" s="196"/>
       <c r="Q20" s="66" t="s">
         <v>2</v>
       </c>
@@ -3440,16 +3513,16 @@
       <c r="U20" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="V20" s="88" t="s">
+      <c r="V20" s="198" t="s">
         <v>2</v>
       </c>
-      <c r="W20" s="86"/>
-      <c r="X20" s="86"/>
-      <c r="Y20" s="86"/>
-      <c r="Z20" s="86"/>
-      <c r="AA20" s="86"/>
-      <c r="AB20" s="86"/>
-      <c r="AC20" s="89"/>
+      <c r="W20" s="196"/>
+      <c r="X20" s="196"/>
+      <c r="Y20" s="196"/>
+      <c r="Z20" s="196"/>
+      <c r="AA20" s="196"/>
+      <c r="AB20" s="196"/>
+      <c r="AC20" s="199"/>
       <c r="AD20" s="28"/>
       <c r="AE20" s="15"/>
       <c r="AF20" s="15"/>
@@ -3466,16 +3539,16 @@
       <c r="F21" s="78"/>
       <c r="G21" s="78"/>
       <c r="H21" s="79"/>
-      <c r="I21" s="87" t="s">
+      <c r="I21" s="197" t="s">
         <v>88</v>
       </c>
-      <c r="J21" s="87"/>
-      <c r="K21" s="87"/>
-      <c r="L21" s="87"/>
-      <c r="M21" s="87"/>
-      <c r="N21" s="87"/>
-      <c r="O21" s="87"/>
-      <c r="P21" s="87"/>
+      <c r="J21" s="197"/>
+      <c r="K21" s="197"/>
+      <c r="L21" s="197"/>
+      <c r="M21" s="197"/>
+      <c r="N21" s="197"/>
+      <c r="O21" s="197"/>
+      <c r="P21" s="197"/>
       <c r="Q21" s="67" t="s">
         <v>88</v>
       </c>
@@ -3489,16 +3562,16 @@
       <c r="U21" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="V21" s="90" t="s">
+      <c r="V21" s="200" t="s">
         <v>89</v>
       </c>
-      <c r="W21" s="91"/>
-      <c r="X21" s="91"/>
-      <c r="Y21" s="91"/>
-      <c r="Z21" s="91"/>
-      <c r="AA21" s="91"/>
-      <c r="AB21" s="91"/>
-      <c r="AC21" s="92"/>
+      <c r="W21" s="201"/>
+      <c r="X21" s="201"/>
+      <c r="Y21" s="201"/>
+      <c r="Z21" s="201"/>
+      <c r="AA21" s="201"/>
+      <c r="AB21" s="201"/>
+      <c r="AC21" s="202"/>
       <c r="AD21" s="43"/>
       <c r="AE21" s="44"/>
       <c r="AF21" s="44"/>
@@ -3508,246 +3581,246 @@
       <c r="AJ21" s="46"/>
     </row>
     <row r="23" spans="2:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H23" s="99" t="s">
+      <c r="H23" s="139" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="135"/>
-      <c r="J23" s="100"/>
-      <c r="L23" s="115" t="s">
+      <c r="I23" s="140"/>
+      <c r="J23" s="141"/>
+      <c r="L23" s="179" t="s">
         <v>48</v>
       </c>
-      <c r="M23" s="116"/>
-      <c r="N23" s="116"/>
-      <c r="O23" s="116"/>
-      <c r="P23" s="116"/>
-      <c r="Q23" s="117"/>
-      <c r="S23" s="99" t="s">
+      <c r="M23" s="180"/>
+      <c r="N23" s="180"/>
+      <c r="O23" s="180"/>
+      <c r="P23" s="180"/>
+      <c r="Q23" s="181"/>
+      <c r="S23" s="139" t="s">
         <v>40</v>
       </c>
-      <c r="T23" s="100"/>
-      <c r="W23" s="125" t="s">
+      <c r="T23" s="141"/>
+      <c r="W23" s="155" t="s">
         <v>34</v>
       </c>
-      <c r="X23" s="126"/>
-      <c r="Y23" s="126"/>
-      <c r="Z23" s="126"/>
-      <c r="AA23" s="126"/>
-      <c r="AB23" s="126"/>
-      <c r="AC23" s="126"/>
-      <c r="AD23" s="127"/>
+      <c r="X23" s="156"/>
+      <c r="Y23" s="156"/>
+      <c r="Z23" s="156"/>
+      <c r="AA23" s="156"/>
+      <c r="AB23" s="156"/>
+      <c r="AC23" s="156"/>
+      <c r="AD23" s="157"/>
     </row>
     <row r="24" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="H24" s="136" t="s">
+      <c r="H24" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="I24" s="137"/>
-      <c r="J24" s="138"/>
-      <c r="L24" s="118"/>
-      <c r="M24" s="119"/>
-      <c r="N24" s="119"/>
-      <c r="O24" s="119"/>
-      <c r="P24" s="119"/>
-      <c r="Q24" s="120"/>
-      <c r="S24" s="101" t="s">
+      <c r="I24" s="143"/>
+      <c r="J24" s="144"/>
+      <c r="L24" s="182"/>
+      <c r="M24" s="183"/>
+      <c r="N24" s="183"/>
+      <c r="O24" s="183"/>
+      <c r="P24" s="183"/>
+      <c r="Q24" s="184"/>
+      <c r="S24" s="166" t="s">
         <v>42</v>
       </c>
-      <c r="T24" s="102"/>
+      <c r="T24" s="167"/>
       <c r="W24" s="8" t="s">
         <v>23</v>
       </c>
       <c r="X24" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="Y24" s="128" t="s">
+      <c r="Y24" s="158" t="s">
         <v>51</v>
       </c>
-      <c r="Z24" s="128"/>
-      <c r="AA24" s="128"/>
-      <c r="AB24" s="128"/>
-      <c r="AC24" s="128"/>
-      <c r="AD24" s="129"/>
+      <c r="Z24" s="158"/>
+      <c r="AA24" s="158"/>
+      <c r="AB24" s="158"/>
+      <c r="AC24" s="158"/>
+      <c r="AD24" s="159"/>
     </row>
     <row r="25" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="H25" s="139" t="s">
+      <c r="H25" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="140"/>
-      <c r="J25" s="141"/>
-      <c r="L25" s="148" t="s">
+      <c r="I25" s="186"/>
+      <c r="J25" s="187"/>
+      <c r="L25" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="M25" s="149"/>
-      <c r="N25" s="149"/>
-      <c r="O25" s="149"/>
-      <c r="P25" s="149"/>
-      <c r="Q25" s="150"/>
-      <c r="S25" s="103" t="s">
+      <c r="M25" s="118"/>
+      <c r="N25" s="118"/>
+      <c r="O25" s="118"/>
+      <c r="P25" s="118"/>
+      <c r="Q25" s="119"/>
+      <c r="S25" s="168" t="s">
         <v>41</v>
       </c>
-      <c r="T25" s="104"/>
+      <c r="T25" s="169"/>
       <c r="W25" s="1" t="s">
         <v>20</v>
       </c>
       <c r="X25" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y25" s="121" t="s">
+      <c r="Y25" s="151" t="s">
         <v>10</v>
       </c>
-      <c r="Z25" s="121"/>
-      <c r="AA25" s="121"/>
-      <c r="AB25" s="121"/>
-      <c r="AC25" s="121"/>
-      <c r="AD25" s="122"/>
+      <c r="Z25" s="151"/>
+      <c r="AA25" s="151"/>
+      <c r="AB25" s="151"/>
+      <c r="AC25" s="151"/>
+      <c r="AD25" s="152"/>
     </row>
     <row r="26" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="H26" s="142" t="s">
+      <c r="H26" s="188" t="s">
         <v>73</v>
       </c>
-      <c r="I26" s="143"/>
-      <c r="J26" s="144"/>
-      <c r="L26" s="111" t="s">
+      <c r="I26" s="189"/>
+      <c r="J26" s="190"/>
+      <c r="L26" s="176" t="s">
         <v>47</v>
       </c>
-      <c r="M26" s="112"/>
-      <c r="N26" s="112"/>
-      <c r="O26" s="112"/>
-      <c r="P26" s="112"/>
-      <c r="Q26" s="113"/>
-      <c r="S26" s="105" t="s">
+      <c r="M26" s="177"/>
+      <c r="N26" s="177"/>
+      <c r="O26" s="177"/>
+      <c r="P26" s="177"/>
+      <c r="Q26" s="178"/>
+      <c r="S26" s="170" t="s">
         <v>13</v>
       </c>
-      <c r="T26" s="106"/>
+      <c r="T26" s="171"/>
       <c r="W26" s="13" t="s">
         <v>33</v>
       </c>
       <c r="X26" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y26" s="121" t="s">
+      <c r="Y26" s="151" t="s">
         <v>50</v>
       </c>
-      <c r="Z26" s="121"/>
-      <c r="AA26" s="121"/>
-      <c r="AB26" s="121"/>
-      <c r="AC26" s="121"/>
-      <c r="AD26" s="122"/>
+      <c r="Z26" s="151"/>
+      <c r="AA26" s="151"/>
+      <c r="AB26" s="151"/>
+      <c r="AC26" s="151"/>
+      <c r="AD26" s="152"/>
     </row>
     <row r="27" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="H27" s="145" t="s">
+      <c r="H27" s="191" t="s">
         <v>39</v>
       </c>
-      <c r="I27" s="146"/>
-      <c r="J27" s="147"/>
-      <c r="L27" s="114"/>
-      <c r="M27" s="114"/>
-      <c r="N27" s="114"/>
-      <c r="O27" s="114"/>
-      <c r="P27" s="114"/>
-      <c r="Q27" s="114"/>
-      <c r="S27" s="107" t="s">
+      <c r="I27" s="192"/>
+      <c r="J27" s="193"/>
+      <c r="L27" s="89"/>
+      <c r="M27" s="89"/>
+      <c r="N27" s="89"/>
+      <c r="O27" s="89"/>
+      <c r="P27" s="89"/>
+      <c r="Q27" s="89"/>
+      <c r="S27" s="172" t="s">
         <v>14</v>
       </c>
-      <c r="T27" s="108"/>
+      <c r="T27" s="173"/>
       <c r="W27" s="9">
         <v>0</v>
       </c>
       <c r="X27" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="Y27" s="123" t="s">
+      <c r="Y27" s="153" t="s">
         <v>32</v>
       </c>
-      <c r="Z27" s="123"/>
-      <c r="AA27" s="123"/>
-      <c r="AB27" s="123"/>
-      <c r="AC27" s="123"/>
-      <c r="AD27" s="124"/>
+      <c r="Z27" s="153"/>
+      <c r="AA27" s="153"/>
+      <c r="AB27" s="153"/>
+      <c r="AC27" s="153"/>
+      <c r="AD27" s="154"/>
     </row>
     <row r="28" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="H28" s="96" t="s">
+      <c r="H28" s="163" t="s">
         <v>43</v>
       </c>
-      <c r="I28" s="97"/>
-      <c r="J28" s="98"/>
-      <c r="L28" s="115" t="s">
+      <c r="I28" s="164"/>
+      <c r="J28" s="165"/>
+      <c r="L28" s="179" t="s">
         <v>49</v>
       </c>
-      <c r="M28" s="116"/>
-      <c r="N28" s="116"/>
-      <c r="O28" s="116"/>
-      <c r="P28" s="116"/>
-      <c r="Q28" s="117"/>
-      <c r="S28" s="109" t="s">
+      <c r="M28" s="180"/>
+      <c r="N28" s="180"/>
+      <c r="O28" s="180"/>
+      <c r="P28" s="180"/>
+      <c r="Q28" s="181"/>
+      <c r="S28" s="174" t="s">
         <v>24</v>
       </c>
-      <c r="T28" s="110"/>
+      <c r="T28" s="175"/>
     </row>
     <row r="29" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="L29" s="118"/>
-      <c r="M29" s="119"/>
-      <c r="N29" s="119"/>
-      <c r="O29" s="119"/>
-      <c r="P29" s="119"/>
-      <c r="Q29" s="120"/>
-      <c r="W29" s="125" t="s">
+      <c r="L29" s="182"/>
+      <c r="M29" s="183"/>
+      <c r="N29" s="183"/>
+      <c r="O29" s="183"/>
+      <c r="P29" s="183"/>
+      <c r="Q29" s="184"/>
+      <c r="W29" s="155" t="s">
         <v>30</v>
       </c>
-      <c r="X29" s="126"/>
-      <c r="Y29" s="126"/>
-      <c r="Z29" s="126"/>
-      <c r="AA29" s="126"/>
-      <c r="AB29" s="126"/>
-      <c r="AC29" s="126"/>
-      <c r="AD29" s="127"/>
+      <c r="X29" s="156"/>
+      <c r="Y29" s="156"/>
+      <c r="Z29" s="156"/>
+      <c r="AA29" s="156"/>
+      <c r="AB29" s="156"/>
+      <c r="AC29" s="156"/>
+      <c r="AD29" s="157"/>
     </row>
     <row r="30" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="L30" s="93" t="s">
+      <c r="L30" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="M30" s="94"/>
-      <c r="N30" s="94"/>
-      <c r="O30" s="94"/>
-      <c r="P30" s="94"/>
-      <c r="Q30" s="95"/>
+      <c r="M30" s="161"/>
+      <c r="N30" s="161"/>
+      <c r="O30" s="161"/>
+      <c r="P30" s="161"/>
+      <c r="Q30" s="162"/>
       <c r="W30" s="4" t="s">
         <v>21</v>
       </c>
       <c r="X30" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="Y30" s="121" t="s">
+      <c r="Y30" s="151" t="s">
         <v>27</v>
       </c>
-      <c r="Z30" s="121"/>
-      <c r="AA30" s="121"/>
-      <c r="AB30" s="121"/>
-      <c r="AC30" s="121"/>
-      <c r="AD30" s="122"/>
+      <c r="Z30" s="151"/>
+      <c r="AA30" s="151"/>
+      <c r="AB30" s="151"/>
+      <c r="AC30" s="151"/>
+      <c r="AD30" s="152"/>
     </row>
     <row r="31" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="L31" s="96" t="s">
+      <c r="L31" s="163" t="s">
         <v>44</v>
       </c>
-      <c r="M31" s="97"/>
-      <c r="N31" s="97"/>
-      <c r="O31" s="97"/>
-      <c r="P31" s="97"/>
-      <c r="Q31" s="98"/>
+      <c r="M31" s="164"/>
+      <c r="N31" s="164"/>
+      <c r="O31" s="164"/>
+      <c r="P31" s="164"/>
+      <c r="Q31" s="165"/>
       <c r="W31" s="6" t="s">
         <v>25</v>
       </c>
       <c r="X31" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="Y31" s="121" t="s">
+      <c r="Y31" s="151" t="s">
         <v>26</v>
       </c>
-      <c r="Z31" s="121"/>
-      <c r="AA31" s="121"/>
-      <c r="AB31" s="121"/>
-      <c r="AC31" s="121"/>
-      <c r="AD31" s="122"/>
+      <c r="Z31" s="151"/>
+      <c r="AA31" s="151"/>
+      <c r="AB31" s="151"/>
+      <c r="AC31" s="151"/>
+      <c r="AD31" s="152"/>
     </row>
     <row r="32" spans="2:36" x14ac:dyDescent="0.25">
       <c r="W32" s="8" t="s">
@@ -3756,14 +3829,14 @@
       <c r="X32" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="Y32" s="121" t="s">
+      <c r="Y32" s="151" t="s">
         <v>28</v>
       </c>
-      <c r="Z32" s="121"/>
-      <c r="AA32" s="121"/>
-      <c r="AB32" s="121"/>
-      <c r="AC32" s="121"/>
-      <c r="AD32" s="122"/>
+      <c r="Z32" s="151"/>
+      <c r="AA32" s="151"/>
+      <c r="AB32" s="151"/>
+      <c r="AC32" s="151"/>
+      <c r="AD32" s="152"/>
     </row>
     <row r="33" spans="19:30" x14ac:dyDescent="0.25">
       <c r="S33" s="14"/>
@@ -3773,81 +3846,25 @@
       <c r="X33" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Y33" s="123" t="s">
+      <c r="Y33" s="153" t="s">
         <v>29</v>
       </c>
-      <c r="Z33" s="123"/>
-      <c r="AA33" s="123"/>
-      <c r="AB33" s="123"/>
-      <c r="AC33" s="123"/>
-      <c r="AD33" s="124"/>
+      <c r="Z33" s="153"/>
+      <c r="AA33" s="153"/>
+      <c r="AB33" s="153"/>
+      <c r="AC33" s="153"/>
+      <c r="AD33" s="154"/>
     </row>
   </sheetData>
-  <mergeCells count="89">
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="AD12:AJ13"/>
-    <mergeCell ref="AD9:AJ10"/>
-    <mergeCell ref="AD15:AJ16"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="B2:H3"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="AD5:AJ5"/>
-    <mergeCell ref="AD2:AJ3"/>
-    <mergeCell ref="I2:J3"/>
-    <mergeCell ref="AB2:AC3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="L25:Q25"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="H4:AD4"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="AB8:AC8"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AB11:AC11"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB9:AC9"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="Y32:AD32"/>
-    <mergeCell ref="Y33:AD33"/>
-    <mergeCell ref="W23:AD23"/>
-    <mergeCell ref="Y24:AD24"/>
-    <mergeCell ref="Y25:AD25"/>
-    <mergeCell ref="Y26:AD26"/>
-    <mergeCell ref="Y27:AD27"/>
-    <mergeCell ref="W29:AD29"/>
-    <mergeCell ref="Y30:AD30"/>
-    <mergeCell ref="Y31:AD31"/>
+  <mergeCells count="91">
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="I20:P20"/>
+    <mergeCell ref="I21:P21"/>
+    <mergeCell ref="V20:AC20"/>
+    <mergeCell ref="V21:AC21"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="AB10:AC10"/>
     <mergeCell ref="L30:Q30"/>
     <mergeCell ref="L31:Q31"/>
     <mergeCell ref="H28:J28"/>
@@ -3864,15 +3881,73 @@
     <mergeCell ref="H25:J25"/>
     <mergeCell ref="H26:J26"/>
     <mergeCell ref="H27:J27"/>
+    <mergeCell ref="Y32:AD32"/>
+    <mergeCell ref="Y33:AD33"/>
+    <mergeCell ref="W23:AD23"/>
+    <mergeCell ref="Y24:AD24"/>
+    <mergeCell ref="Y25:AD25"/>
+    <mergeCell ref="Y26:AD26"/>
+    <mergeCell ref="Y27:AD27"/>
+    <mergeCell ref="W29:AD29"/>
+    <mergeCell ref="Y30:AD30"/>
+    <mergeCell ref="Y31:AD31"/>
+    <mergeCell ref="AB8:AC8"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AB11:AC11"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB9:AC9"/>
     <mergeCell ref="AB12:AC12"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="I20:P20"/>
-    <mergeCell ref="I21:P21"/>
-    <mergeCell ref="V20:AC20"/>
-    <mergeCell ref="V21:AC21"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="AB10:AC10"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L25:Q25"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="H4:AD4"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="B2:H3"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="AD5:AJ5"/>
+    <mergeCell ref="AD2:AJ3"/>
+    <mergeCell ref="I2:J3"/>
+    <mergeCell ref="AB2:AC3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="AD12:AJ13"/>
+    <mergeCell ref="AD9:AJ10"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AG15:AG16"/>
+    <mergeCell ref="AD15:AF16"/>
+    <mergeCell ref="AH15:AJ16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
+Reformed Main.cpp +Refoemed file structure for Tx classes + add special Msg() for lora with offset +clear file structure
</commit_message>
<xml_diff>
--- a/docks/UFO_Pinout.xlsx
+++ b/docks/UFO_Pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\esppres_my_workspace\UFO_1\docks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48936C9F-3200-47DE-852A-816AC684DBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB079383-C129-46D3-98B5-3FDF2392A80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2235" yWindow="1170" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ESP32 DevKitC v4" sheetId="9" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="108">
   <si>
     <t>EN</t>
   </si>
@@ -327,12 +327,6 @@
   </si>
   <si>
     <t>UART1</t>
-  </si>
-  <si>
-    <t>I2C Software SDA</t>
-  </si>
-  <si>
-    <t>I2C Software SCL</t>
   </si>
   <si>
     <t>UART3</t>
@@ -1598,52 +1592,307 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1691,298 +1940,43 @@
     <xf numFmtId="0" fontId="1" fillId="20" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2272,8 +2266,8 @@
   <sheetPr codeName="Лист9"/>
   <dimension ref="B1:AJ33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AG33" sqref="AG33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2297,165 +2291,165 @@
   <sheetData>
     <row r="1" spans="2:36" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:36" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="183" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="107" t="s">
+      <c r="C2" s="184"/>
+      <c r="D2" s="184"/>
+      <c r="E2" s="184"/>
+      <c r="F2" s="184"/>
+      <c r="G2" s="184"/>
+      <c r="H2" s="185"/>
+      <c r="I2" s="192" t="s">
         <v>85</v>
       </c>
-      <c r="J2" s="108"/>
-      <c r="K2" s="136" t="s">
+      <c r="J2" s="193"/>
+      <c r="K2" s="156" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="122" t="s">
+      <c r="L2" s="163" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="128" t="s">
+      <c r="M2" s="169" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="113" t="s">
+      <c r="N2" s="175" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="115" t="s">
+      <c r="O2" s="171" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="126" t="s">
+      <c r="P2" s="167" t="s">
         <v>86</v>
       </c>
-      <c r="Q2" s="124" t="s">
+      <c r="Q2" s="165" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="120" t="s">
+      <c r="R2" s="161" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="130" t="s">
+      <c r="S2" s="173" t="s">
         <v>92</v>
       </c>
-      <c r="T2" s="132" t="s">
+      <c r="T2" s="177" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="134" t="s">
+      <c r="U2" s="179" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="126" t="s">
+      <c r="V2" s="167" t="s">
         <v>86</v>
       </c>
-      <c r="W2" s="115" t="s">
+      <c r="W2" s="171" t="s">
         <v>15</v>
       </c>
-      <c r="X2" s="113" t="s">
+      <c r="X2" s="175" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" s="128" t="s">
+      <c r="Y2" s="169" t="s">
         <v>31</v>
       </c>
-      <c r="Z2" s="122" t="s">
+      <c r="Z2" s="163" t="s">
         <v>19</v>
       </c>
-      <c r="AA2" s="136" t="s">
+      <c r="AA2" s="156" t="s">
         <v>18</v>
       </c>
-      <c r="AB2" s="111" t="s">
+      <c r="AB2" s="196" t="s">
         <v>85</v>
       </c>
-      <c r="AC2" s="107"/>
-      <c r="AD2" s="98" t="s">
+      <c r="AC2" s="192"/>
+      <c r="AD2" s="183" t="s">
         <v>35</v>
       </c>
-      <c r="AE2" s="99"/>
-      <c r="AF2" s="99"/>
-      <c r="AG2" s="99"/>
-      <c r="AH2" s="99"/>
-      <c r="AI2" s="99"/>
-      <c r="AJ2" s="100"/>
+      <c r="AE2" s="184"/>
+      <c r="AF2" s="184"/>
+      <c r="AG2" s="184"/>
+      <c r="AH2" s="184"/>
+      <c r="AI2" s="184"/>
+      <c r="AJ2" s="185"/>
     </row>
     <row r="3" spans="2:36" s="2" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="101"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="109"/>
-      <c r="J3" s="110"/>
-      <c r="K3" s="137"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="129"/>
-      <c r="N3" s="114"/>
-      <c r="O3" s="116"/>
-      <c r="P3" s="127"/>
-      <c r="Q3" s="125"/>
-      <c r="R3" s="121"/>
-      <c r="S3" s="131"/>
-      <c r="T3" s="133"/>
-      <c r="U3" s="135"/>
-      <c r="V3" s="127"/>
-      <c r="W3" s="116"/>
-      <c r="X3" s="114"/>
-      <c r="Y3" s="129"/>
-      <c r="Z3" s="123"/>
-      <c r="AA3" s="137"/>
-      <c r="AB3" s="112"/>
-      <c r="AC3" s="109"/>
-      <c r="AD3" s="101"/>
-      <c r="AE3" s="102"/>
-      <c r="AF3" s="102"/>
-      <c r="AG3" s="102"/>
-      <c r="AH3" s="102"/>
-      <c r="AI3" s="102"/>
-      <c r="AJ3" s="103"/>
+      <c r="B3" s="186"/>
+      <c r="C3" s="187"/>
+      <c r="D3" s="187"/>
+      <c r="E3" s="187"/>
+      <c r="F3" s="187"/>
+      <c r="G3" s="187"/>
+      <c r="H3" s="188"/>
+      <c r="I3" s="194"/>
+      <c r="J3" s="195"/>
+      <c r="K3" s="157"/>
+      <c r="L3" s="164"/>
+      <c r="M3" s="170"/>
+      <c r="N3" s="176"/>
+      <c r="O3" s="172"/>
+      <c r="P3" s="168"/>
+      <c r="Q3" s="166"/>
+      <c r="R3" s="162"/>
+      <c r="S3" s="174"/>
+      <c r="T3" s="178"/>
+      <c r="U3" s="180"/>
+      <c r="V3" s="168"/>
+      <c r="W3" s="172"/>
+      <c r="X3" s="176"/>
+      <c r="Y3" s="170"/>
+      <c r="Z3" s="164"/>
+      <c r="AA3" s="157"/>
+      <c r="AB3" s="197"/>
+      <c r="AC3" s="194"/>
+      <c r="AD3" s="186"/>
+      <c r="AE3" s="187"/>
+      <c r="AF3" s="187"/>
+      <c r="AG3" s="187"/>
+      <c r="AH3" s="187"/>
+      <c r="AI3" s="187"/>
+      <c r="AJ3" s="188"/>
     </row>
     <row r="4" spans="2:36" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H4" s="138"/>
-      <c r="I4" s="138"/>
-      <c r="J4" s="138"/>
-      <c r="K4" s="138"/>
-      <c r="L4" s="138"/>
-      <c r="M4" s="138"/>
-      <c r="N4" s="138"/>
-      <c r="O4" s="138"/>
-      <c r="P4" s="138"/>
-      <c r="Q4" s="138"/>
-      <c r="R4" s="138"/>
-      <c r="S4" s="138"/>
-      <c r="T4" s="138"/>
-      <c r="U4" s="138"/>
-      <c r="V4" s="138"/>
-      <c r="W4" s="138"/>
-      <c r="X4" s="138"/>
-      <c r="Y4" s="138"/>
-      <c r="Z4" s="138"/>
-      <c r="AA4" s="138"/>
-      <c r="AB4" s="138"/>
-      <c r="AC4" s="138"/>
-      <c r="AD4" s="138"/>
+      <c r="H4" s="181"/>
+      <c r="I4" s="181"/>
+      <c r="J4" s="181"/>
+      <c r="K4" s="181"/>
+      <c r="L4" s="181"/>
+      <c r="M4" s="181"/>
+      <c r="N4" s="181"/>
+      <c r="O4" s="181"/>
+      <c r="P4" s="181"/>
+      <c r="Q4" s="181"/>
+      <c r="R4" s="181"/>
+      <c r="S4" s="181"/>
+      <c r="T4" s="181"/>
+      <c r="U4" s="181"/>
+      <c r="V4" s="181"/>
+      <c r="W4" s="181"/>
+      <c r="X4" s="181"/>
+      <c r="Y4" s="181"/>
+      <c r="Z4" s="181"/>
+      <c r="AA4" s="181"/>
+      <c r="AB4" s="181"/>
+      <c r="AC4" s="181"/>
+      <c r="AD4" s="181"/>
     </row>
     <row r="5" spans="2:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="104" t="s">
+      <c r="B5" s="189" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="105"/>
-      <c r="H5" s="106"/>
-      <c r="AD5" s="104" t="s">
+      <c r="C5" s="190"/>
+      <c r="D5" s="190"/>
+      <c r="E5" s="190"/>
+      <c r="F5" s="190"/>
+      <c r="G5" s="190"/>
+      <c r="H5" s="191"/>
+      <c r="AD5" s="189" t="s">
         <v>87</v>
       </c>
-      <c r="AE5" s="105"/>
-      <c r="AF5" s="105"/>
-      <c r="AG5" s="105"/>
-      <c r="AH5" s="105"/>
-      <c r="AI5" s="105"/>
-      <c r="AJ5" s="106"/>
+      <c r="AE5" s="190"/>
+      <c r="AF5" s="190"/>
+      <c r="AG5" s="190"/>
+      <c r="AH5" s="190"/>
+      <c r="AI5" s="190"/>
+      <c r="AJ5" s="191"/>
     </row>
     <row r="6" spans="2:36" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="50">
@@ -2479,17 +2473,17 @@
       <c r="H6" s="52">
         <v>0</v>
       </c>
-      <c r="AD6" s="203" t="s">
+      <c r="AD6" s="82" t="s">
         <v>97</v>
       </c>
-      <c r="AE6" s="205" t="s">
+      <c r="AE6" s="84" t="s">
         <v>98</v>
       </c>
-      <c r="AF6" s="207" t="s">
+      <c r="AF6" s="86" t="s">
         <v>99</v>
       </c>
-      <c r="AG6" s="210" t="s">
-        <v>108</v>
+      <c r="AG6" s="89" t="s">
+        <v>106</v>
       </c>
       <c r="AH6" s="51">
         <v>4</v>
@@ -2502,17 +2496,17 @@
       </c>
     </row>
     <row r="7" spans="2:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="94"/>
-      <c r="C7" s="95"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="146" t="s">
+      <c r="B7" s="198"/>
+      <c r="C7" s="199"/>
+      <c r="D7" s="199"/>
+      <c r="E7" s="199"/>
+      <c r="F7" s="199"/>
+      <c r="G7" s="199"/>
+      <c r="H7" s="200"/>
+      <c r="I7" s="154" t="s">
         <v>84</v>
       </c>
-      <c r="J7" s="147"/>
+      <c r="J7" s="155"/>
       <c r="K7" s="53" t="s">
         <v>20</v>
       </c>
@@ -2562,10 +2556,10 @@
       <c r="AA7" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="AB7" s="194" t="s">
+      <c r="AB7" s="90" t="s">
         <v>94</v>
       </c>
-      <c r="AC7" s="195"/>
+      <c r="AC7" s="91"/>
       <c r="AD7" s="60"/>
       <c r="AE7" s="42"/>
       <c r="AF7" s="42"/>
@@ -2582,8 +2576,8 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="29"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="97"/>
+      <c r="I8" s="201"/>
+      <c r="J8" s="202"/>
       <c r="K8" s="8" t="s">
         <v>23</v>
       </c>
@@ -2633,17 +2627,17 @@
       <c r="AA8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AB8" s="148" t="s">
+      <c r="AB8" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="AC8" s="84"/>
-      <c r="AD8" s="204" t="s">
+      <c r="AC8" s="100"/>
+      <c r="AD8" s="83" t="s">
         <v>97</v>
       </c>
-      <c r="AE8" s="206" t="s">
+      <c r="AE8" s="85" t="s">
         <v>98</v>
       </c>
-      <c r="AF8" s="208" t="s">
+      <c r="AF8" s="87" t="s">
         <v>99</v>
       </c>
       <c r="AG8" s="15"/>
@@ -2659,8 +2653,8 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="29"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="97"/>
+      <c r="I9" s="201"/>
+      <c r="J9" s="202"/>
       <c r="K9" s="8" t="s">
         <v>23</v>
       </c>
@@ -2710,19 +2704,19 @@
       <c r="AA9" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="AB9" s="149" t="s">
+      <c r="AB9" s="101" t="s">
         <v>76</v>
       </c>
-      <c r="AC9" s="150"/>
-      <c r="AD9" s="88" t="s">
+      <c r="AC9" s="102"/>
+      <c r="AD9" s="206" t="s">
         <v>101</v>
       </c>
-      <c r="AE9" s="89"/>
-      <c r="AF9" s="89"/>
-      <c r="AG9" s="89"/>
-      <c r="AH9" s="89"/>
-      <c r="AI9" s="89"/>
-      <c r="AJ9" s="90"/>
+      <c r="AE9" s="124"/>
+      <c r="AF9" s="124"/>
+      <c r="AG9" s="124"/>
+      <c r="AH9" s="124"/>
+      <c r="AI9" s="124"/>
+      <c r="AJ9" s="207"/>
     </row>
     <row r="10" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B10" s="28"/>
@@ -2732,8 +2726,8 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="29"/>
-      <c r="I10" s="83"/>
-      <c r="J10" s="97"/>
+      <c r="I10" s="201"/>
+      <c r="J10" s="202"/>
       <c r="K10" s="8" t="s">
         <v>23</v>
       </c>
@@ -2783,17 +2777,17 @@
       <c r="AA10" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="AB10" s="149" t="s">
+      <c r="AB10" s="101" t="s">
         <v>77</v>
       </c>
-      <c r="AC10" s="150"/>
-      <c r="AD10" s="91"/>
-      <c r="AE10" s="92"/>
-      <c r="AF10" s="92"/>
-      <c r="AG10" s="92"/>
-      <c r="AH10" s="92"/>
-      <c r="AI10" s="92"/>
-      <c r="AJ10" s="93"/>
+      <c r="AC10" s="102"/>
+      <c r="AD10" s="208"/>
+      <c r="AE10" s="209"/>
+      <c r="AF10" s="209"/>
+      <c r="AG10" s="209"/>
+      <c r="AH10" s="209"/>
+      <c r="AI10" s="209"/>
+      <c r="AJ10" s="210"/>
     </row>
     <row r="11" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B11" s="28"/>
@@ -2803,8 +2797,8 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="29"/>
-      <c r="I11" s="83"/>
-      <c r="J11" s="97"/>
+      <c r="I11" s="201"/>
+      <c r="J11" s="202"/>
       <c r="K11" s="8" t="s">
         <v>23</v>
       </c>
@@ -2854,17 +2848,17 @@
       <c r="AA11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AB11" s="148" t="s">
+      <c r="AB11" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="AC11" s="84"/>
-      <c r="AD11" s="204" t="s">
+      <c r="AC11" s="100"/>
+      <c r="AD11" s="83" t="s">
         <v>97</v>
       </c>
-      <c r="AE11" s="206" t="s">
+      <c r="AE11" s="85" t="s">
         <v>98</v>
       </c>
-      <c r="AF11" s="208" t="s">
+      <c r="AF11" s="87" t="s">
         <v>99</v>
       </c>
       <c r="AG11" s="15"/>
@@ -2873,17 +2867,15 @@
       <c r="AJ11" s="29"/>
     </row>
     <row r="12" spans="2:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="85" t="s">
-        <v>102</v>
-      </c>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="87"/>
-      <c r="I12" s="83"/>
-      <c r="J12" s="97"/>
+      <c r="B12" s="204"/>
+      <c r="C12" s="152"/>
+      <c r="D12" s="152"/>
+      <c r="E12" s="152"/>
+      <c r="F12" s="152"/>
+      <c r="G12" s="152"/>
+      <c r="H12" s="205"/>
+      <c r="I12" s="201"/>
+      <c r="J12" s="202"/>
       <c r="K12" s="8" t="s">
         <v>23</v>
       </c>
@@ -2933,32 +2925,30 @@
       <c r="AA12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AB12" s="148" t="s">
+      <c r="AB12" s="99" t="s">
         <v>95</v>
       </c>
-      <c r="AC12" s="84"/>
-      <c r="AD12" s="88" t="s">
-        <v>104</v>
-      </c>
-      <c r="AE12" s="89"/>
-      <c r="AF12" s="89"/>
-      <c r="AG12" s="89"/>
-      <c r="AH12" s="89"/>
-      <c r="AI12" s="89"/>
-      <c r="AJ12" s="90"/>
+      <c r="AC12" s="100"/>
+      <c r="AD12" s="206" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE12" s="124"/>
+      <c r="AF12" s="124"/>
+      <c r="AG12" s="124"/>
+      <c r="AH12" s="124"/>
+      <c r="AI12" s="124"/>
+      <c r="AJ12" s="207"/>
     </row>
     <row r="13" spans="2:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="85" t="s">
-        <v>103</v>
-      </c>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="83"/>
-      <c r="J13" s="97"/>
+      <c r="B13" s="204"/>
+      <c r="C13" s="152"/>
+      <c r="D13" s="152"/>
+      <c r="E13" s="152"/>
+      <c r="F13" s="152"/>
+      <c r="G13" s="152"/>
+      <c r="H13" s="205"/>
+      <c r="I13" s="201"/>
+      <c r="J13" s="202"/>
       <c r="K13" s="8" t="s">
         <v>23</v>
       </c>
@@ -3008,17 +2998,17 @@
       <c r="AA13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AB13" s="148" t="s">
+      <c r="AB13" s="99" t="s">
         <v>96</v>
       </c>
-      <c r="AC13" s="84"/>
-      <c r="AD13" s="91"/>
-      <c r="AE13" s="92"/>
-      <c r="AF13" s="92"/>
-      <c r="AG13" s="92"/>
-      <c r="AH13" s="92"/>
-      <c r="AI13" s="92"/>
-      <c r="AJ13" s="93"/>
+      <c r="AC13" s="100"/>
+      <c r="AD13" s="208"/>
+      <c r="AE13" s="209"/>
+      <c r="AF13" s="209"/>
+      <c r="AG13" s="209"/>
+      <c r="AH13" s="209"/>
+      <c r="AI13" s="209"/>
+      <c r="AJ13" s="210"/>
     </row>
     <row r="14" spans="2:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="28"/>
@@ -3028,10 +3018,10 @@
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
       <c r="H14" s="29"/>
-      <c r="I14" s="86" t="s">
+      <c r="I14" s="152" t="s">
         <v>82</v>
       </c>
-      <c r="J14" s="145"/>
+      <c r="J14" s="153"/>
       <c r="K14" s="8" t="s">
         <v>23</v>
       </c>
@@ -3081,34 +3071,34 @@
       <c r="AA14" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="AB14" s="148" t="s">
+      <c r="AB14" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="AC14" s="84"/>
+      <c r="AC14" s="100"/>
       <c r="AD14" s="28"/>
       <c r="AE14" s="15"/>
       <c r="AF14" s="15"/>
-      <c r="AG14" s="209" t="s">
-        <v>105</v>
+      <c r="AG14" s="88" t="s">
+        <v>103</v>
       </c>
       <c r="AH14" s="15"/>
       <c r="AI14" s="15"/>
       <c r="AJ14" s="29"/>
     </row>
     <row r="15" spans="2:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="82" t="s">
+      <c r="B15" s="203" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="83"/>
-      <c r="F15" s="83"/>
-      <c r="G15" s="83"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="86" t="s">
+      <c r="C15" s="201"/>
+      <c r="D15" s="201"/>
+      <c r="E15" s="201"/>
+      <c r="F15" s="201"/>
+      <c r="G15" s="201"/>
+      <c r="H15" s="100"/>
+      <c r="I15" s="152" t="s">
         <v>83</v>
       </c>
-      <c r="J15" s="145"/>
+      <c r="J15" s="153"/>
       <c r="K15" s="8" t="s">
         <v>23</v>
       </c>
@@ -3158,36 +3148,36 @@
       <c r="AA15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AB15" s="148" t="s">
+      <c r="AB15" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="AC15" s="84"/>
-      <c r="AD15" s="88" t="s">
+      <c r="AC15" s="100"/>
+      <c r="AD15" s="206" t="s">
         <v>100</v>
       </c>
-      <c r="AE15" s="89"/>
-      <c r="AF15" s="89"/>
+      <c r="AE15" s="124"/>
+      <c r="AF15" s="124"/>
       <c r="AG15" s="211" t="s">
-        <v>109</v>
-      </c>
-      <c r="AH15" s="88" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH15" s="206" t="s">
         <v>100</v>
       </c>
-      <c r="AI15" s="89"/>
-      <c r="AJ15" s="89"/>
+      <c r="AI15" s="124"/>
+      <c r="AJ15" s="124"/>
     </row>
     <row r="16" spans="2:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="82" t="s">
+      <c r="B16" s="203" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="83"/>
-      <c r="D16" s="83"/>
-      <c r="E16" s="83"/>
-      <c r="F16" s="83"/>
-      <c r="G16" s="83"/>
-      <c r="H16" s="84"/>
-      <c r="I16" s="83"/>
-      <c r="J16" s="97"/>
+      <c r="C16" s="201"/>
+      <c r="D16" s="201"/>
+      <c r="E16" s="201"/>
+      <c r="F16" s="201"/>
+      <c r="G16" s="201"/>
+      <c r="H16" s="100"/>
+      <c r="I16" s="201"/>
+      <c r="J16" s="202"/>
       <c r="K16" s="8" t="s">
         <v>23</v>
       </c>
@@ -3237,28 +3227,28 @@
       <c r="AA16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AB16" s="148" t="s">
+      <c r="AB16" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="AC16" s="84"/>
-      <c r="AD16" s="91"/>
-      <c r="AE16" s="92"/>
-      <c r="AF16" s="92"/>
+      <c r="AC16" s="100"/>
+      <c r="AD16" s="208"/>
+      <c r="AE16" s="209"/>
+      <c r="AF16" s="209"/>
       <c r="AG16" s="212"/>
-      <c r="AH16" s="91"/>
-      <c r="AI16" s="92"/>
-      <c r="AJ16" s="92"/>
+      <c r="AH16" s="208"/>
+      <c r="AI16" s="209"/>
+      <c r="AJ16" s="209"/>
     </row>
     <row r="17" spans="2:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="82" t="s">
+      <c r="B17" s="203" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="83"/>
-      <c r="D17" s="83"/>
-      <c r="E17" s="83"/>
-      <c r="F17" s="83"/>
-      <c r="G17" s="83"/>
-      <c r="H17" s="84"/>
+      <c r="C17" s="201"/>
+      <c r="D17" s="201"/>
+      <c r="E17" s="201"/>
+      <c r="F17" s="201"/>
+      <c r="G17" s="201"/>
+      <c r="H17" s="100"/>
       <c r="I17" s="38" t="s">
         <v>78</v>
       </c>
@@ -3314,13 +3304,13 @@
       <c r="AA17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AB17" s="148"/>
-      <c r="AC17" s="84"/>
+      <c r="AB17" s="99"/>
+      <c r="AC17" s="100"/>
       <c r="AD17" s="28"/>
       <c r="AE17" s="15"/>
       <c r="AF17" s="15"/>
-      <c r="AG17" s="209" t="s">
-        <v>107</v>
+      <c r="AG17" s="88" t="s">
+        <v>105</v>
       </c>
       <c r="AH17" s="15"/>
       <c r="AI17" s="15"/>
@@ -3389,30 +3379,30 @@
       <c r="AA18" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="AB18" s="148" t="s">
+      <c r="AB18" s="99" t="s">
         <v>90</v>
       </c>
-      <c r="AC18" s="84"/>
+      <c r="AC18" s="100"/>
       <c r="AD18" s="28"/>
       <c r="AE18" s="15"/>
       <c r="AF18" s="15"/>
-      <c r="AG18" s="209" t="s">
-        <v>106</v>
+      <c r="AG18" s="88" t="s">
+        <v>104</v>
       </c>
       <c r="AH18" s="15"/>
       <c r="AI18" s="15"/>
       <c r="AJ18" s="29"/>
     </row>
     <row r="19" spans="2:36" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="82" t="s">
+      <c r="B19" s="203" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="83"/>
-      <c r="D19" s="83"/>
-      <c r="E19" s="83"/>
-      <c r="F19" s="83"/>
-      <c r="G19" s="83"/>
-      <c r="H19" s="84"/>
+      <c r="C19" s="201"/>
+      <c r="D19" s="201"/>
+      <c r="E19" s="201"/>
+      <c r="F19" s="201"/>
+      <c r="G19" s="201"/>
+      <c r="H19" s="100"/>
       <c r="I19" s="38" t="s">
         <v>80</v>
       </c>
@@ -3490,16 +3480,16 @@
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="29"/>
-      <c r="I20" s="196" t="s">
+      <c r="I20" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="J20" s="196"/>
-      <c r="K20" s="196"/>
-      <c r="L20" s="196"/>
-      <c r="M20" s="196"/>
-      <c r="N20" s="196"/>
-      <c r="O20" s="196"/>
-      <c r="P20" s="196"/>
+      <c r="J20" s="92"/>
+      <c r="K20" s="92"/>
+      <c r="L20" s="92"/>
+      <c r="M20" s="92"/>
+      <c r="N20" s="92"/>
+      <c r="O20" s="92"/>
+      <c r="P20" s="92"/>
       <c r="Q20" s="66" t="s">
         <v>2</v>
       </c>
@@ -3513,16 +3503,16 @@
       <c r="U20" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="V20" s="198" t="s">
+      <c r="V20" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="W20" s="196"/>
-      <c r="X20" s="196"/>
-      <c r="Y20" s="196"/>
-      <c r="Z20" s="196"/>
-      <c r="AA20" s="196"/>
-      <c r="AB20" s="196"/>
-      <c r="AC20" s="199"/>
+      <c r="W20" s="92"/>
+      <c r="X20" s="92"/>
+      <c r="Y20" s="92"/>
+      <c r="Z20" s="92"/>
+      <c r="AA20" s="92"/>
+      <c r="AB20" s="92"/>
+      <c r="AC20" s="95"/>
       <c r="AD20" s="28"/>
       <c r="AE20" s="15"/>
       <c r="AF20" s="15"/>
@@ -3539,16 +3529,16 @@
       <c r="F21" s="78"/>
       <c r="G21" s="78"/>
       <c r="H21" s="79"/>
-      <c r="I21" s="197" t="s">
+      <c r="I21" s="93" t="s">
         <v>88</v>
       </c>
-      <c r="J21" s="197"/>
-      <c r="K21" s="197"/>
-      <c r="L21" s="197"/>
-      <c r="M21" s="197"/>
-      <c r="N21" s="197"/>
-      <c r="O21" s="197"/>
-      <c r="P21" s="197"/>
+      <c r="J21" s="93"/>
+      <c r="K21" s="93"/>
+      <c r="L21" s="93"/>
+      <c r="M21" s="93"/>
+      <c r="N21" s="93"/>
+      <c r="O21" s="93"/>
+      <c r="P21" s="93"/>
       <c r="Q21" s="67" t="s">
         <v>88</v>
       </c>
@@ -3562,16 +3552,16 @@
       <c r="U21" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="V21" s="200" t="s">
+      <c r="V21" s="96" t="s">
         <v>89</v>
       </c>
-      <c r="W21" s="201"/>
-      <c r="X21" s="201"/>
-      <c r="Y21" s="201"/>
-      <c r="Z21" s="201"/>
-      <c r="AA21" s="201"/>
-      <c r="AB21" s="201"/>
-      <c r="AC21" s="202"/>
+      <c r="W21" s="97"/>
+      <c r="X21" s="97"/>
+      <c r="Y21" s="97"/>
+      <c r="Z21" s="97"/>
+      <c r="AA21" s="97"/>
+      <c r="AB21" s="97"/>
+      <c r="AC21" s="98"/>
       <c r="AD21" s="43"/>
       <c r="AE21" s="44"/>
       <c r="AF21" s="44"/>
@@ -3581,246 +3571,246 @@
       <c r="AJ21" s="46"/>
     </row>
     <row r="23" spans="2:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H23" s="139" t="s">
+      <c r="H23" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="140"/>
-      <c r="J23" s="141"/>
-      <c r="L23" s="179" t="s">
+      <c r="I23" s="182"/>
+      <c r="J23" s="110"/>
+      <c r="L23" s="125" t="s">
         <v>48</v>
       </c>
-      <c r="M23" s="180"/>
-      <c r="N23" s="180"/>
-      <c r="O23" s="180"/>
-      <c r="P23" s="180"/>
-      <c r="Q23" s="181"/>
-      <c r="S23" s="139" t="s">
+      <c r="M23" s="126"/>
+      <c r="N23" s="126"/>
+      <c r="O23" s="126"/>
+      <c r="P23" s="126"/>
+      <c r="Q23" s="127"/>
+      <c r="S23" s="109" t="s">
         <v>40</v>
       </c>
-      <c r="T23" s="141"/>
-      <c r="W23" s="155" t="s">
+      <c r="T23" s="110"/>
+      <c r="W23" s="144" t="s">
         <v>34</v>
       </c>
-      <c r="X23" s="156"/>
-      <c r="Y23" s="156"/>
-      <c r="Z23" s="156"/>
-      <c r="AA23" s="156"/>
-      <c r="AB23" s="156"/>
-      <c r="AC23" s="156"/>
-      <c r="AD23" s="157"/>
+      <c r="X23" s="145"/>
+      <c r="Y23" s="145"/>
+      <c r="Z23" s="145"/>
+      <c r="AA23" s="145"/>
+      <c r="AB23" s="145"/>
+      <c r="AC23" s="145"/>
+      <c r="AD23" s="146"/>
     </row>
     <row r="24" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="H24" s="142" t="s">
+      <c r="H24" s="149" t="s">
         <v>11</v>
       </c>
-      <c r="I24" s="143"/>
-      <c r="J24" s="144"/>
-      <c r="L24" s="182"/>
-      <c r="M24" s="183"/>
-      <c r="N24" s="183"/>
-      <c r="O24" s="183"/>
-      <c r="P24" s="183"/>
-      <c r="Q24" s="184"/>
-      <c r="S24" s="166" t="s">
+      <c r="I24" s="150"/>
+      <c r="J24" s="151"/>
+      <c r="L24" s="128"/>
+      <c r="M24" s="129"/>
+      <c r="N24" s="129"/>
+      <c r="O24" s="129"/>
+      <c r="P24" s="129"/>
+      <c r="Q24" s="130"/>
+      <c r="S24" s="111" t="s">
         <v>42</v>
       </c>
-      <c r="T24" s="167"/>
+      <c r="T24" s="112"/>
       <c r="W24" s="8" t="s">
         <v>23</v>
       </c>
       <c r="X24" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="Y24" s="158" t="s">
+      <c r="Y24" s="147" t="s">
         <v>51</v>
       </c>
-      <c r="Z24" s="158"/>
-      <c r="AA24" s="158"/>
-      <c r="AB24" s="158"/>
-      <c r="AC24" s="158"/>
-      <c r="AD24" s="159"/>
+      <c r="Z24" s="147"/>
+      <c r="AA24" s="147"/>
+      <c r="AB24" s="147"/>
+      <c r="AC24" s="147"/>
+      <c r="AD24" s="148"/>
     </row>
     <row r="25" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="H25" s="185" t="s">
+      <c r="H25" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="186"/>
-      <c r="J25" s="187"/>
-      <c r="L25" s="117" t="s">
+      <c r="I25" s="132"/>
+      <c r="J25" s="133"/>
+      <c r="L25" s="158" t="s">
         <v>46</v>
       </c>
-      <c r="M25" s="118"/>
-      <c r="N25" s="118"/>
-      <c r="O25" s="118"/>
-      <c r="P25" s="118"/>
-      <c r="Q25" s="119"/>
-      <c r="S25" s="168" t="s">
+      <c r="M25" s="159"/>
+      <c r="N25" s="159"/>
+      <c r="O25" s="159"/>
+      <c r="P25" s="159"/>
+      <c r="Q25" s="160"/>
+      <c r="S25" s="113" t="s">
         <v>41</v>
       </c>
-      <c r="T25" s="169"/>
+      <c r="T25" s="114"/>
       <c r="W25" s="1" t="s">
         <v>20</v>
       </c>
       <c r="X25" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y25" s="151" t="s">
+      <c r="Y25" s="140" t="s">
         <v>10</v>
       </c>
-      <c r="Z25" s="151"/>
-      <c r="AA25" s="151"/>
-      <c r="AB25" s="151"/>
-      <c r="AC25" s="151"/>
-      <c r="AD25" s="152"/>
+      <c r="Z25" s="140"/>
+      <c r="AA25" s="140"/>
+      <c r="AB25" s="140"/>
+      <c r="AC25" s="140"/>
+      <c r="AD25" s="141"/>
     </row>
     <row r="26" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="H26" s="188" t="s">
+      <c r="H26" s="134" t="s">
         <v>73</v>
       </c>
-      <c r="I26" s="189"/>
-      <c r="J26" s="190"/>
-      <c r="L26" s="176" t="s">
+      <c r="I26" s="135"/>
+      <c r="J26" s="136"/>
+      <c r="L26" s="121" t="s">
         <v>47</v>
       </c>
-      <c r="M26" s="177"/>
-      <c r="N26" s="177"/>
-      <c r="O26" s="177"/>
-      <c r="P26" s="177"/>
-      <c r="Q26" s="178"/>
-      <c r="S26" s="170" t="s">
+      <c r="M26" s="122"/>
+      <c r="N26" s="122"/>
+      <c r="O26" s="122"/>
+      <c r="P26" s="122"/>
+      <c r="Q26" s="123"/>
+      <c r="S26" s="115" t="s">
         <v>13</v>
       </c>
-      <c r="T26" s="171"/>
+      <c r="T26" s="116"/>
       <c r="W26" s="13" t="s">
         <v>33</v>
       </c>
       <c r="X26" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y26" s="151" t="s">
+      <c r="Y26" s="140" t="s">
         <v>50</v>
       </c>
-      <c r="Z26" s="151"/>
-      <c r="AA26" s="151"/>
-      <c r="AB26" s="151"/>
-      <c r="AC26" s="151"/>
-      <c r="AD26" s="152"/>
+      <c r="Z26" s="140"/>
+      <c r="AA26" s="140"/>
+      <c r="AB26" s="140"/>
+      <c r="AC26" s="140"/>
+      <c r="AD26" s="141"/>
     </row>
     <row r="27" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="H27" s="191" t="s">
+      <c r="H27" s="137" t="s">
         <v>39</v>
       </c>
-      <c r="I27" s="192"/>
-      <c r="J27" s="193"/>
-      <c r="L27" s="89"/>
-      <c r="M27" s="89"/>
-      <c r="N27" s="89"/>
-      <c r="O27" s="89"/>
-      <c r="P27" s="89"/>
-      <c r="Q27" s="89"/>
-      <c r="S27" s="172" t="s">
+      <c r="I27" s="138"/>
+      <c r="J27" s="139"/>
+      <c r="L27" s="124"/>
+      <c r="M27" s="124"/>
+      <c r="N27" s="124"/>
+      <c r="O27" s="124"/>
+      <c r="P27" s="124"/>
+      <c r="Q27" s="124"/>
+      <c r="S27" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="T27" s="173"/>
+      <c r="T27" s="118"/>
       <c r="W27" s="9">
         <v>0</v>
       </c>
       <c r="X27" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="Y27" s="153" t="s">
+      <c r="Y27" s="142" t="s">
         <v>32</v>
       </c>
-      <c r="Z27" s="153"/>
-      <c r="AA27" s="153"/>
-      <c r="AB27" s="153"/>
-      <c r="AC27" s="153"/>
-      <c r="AD27" s="154"/>
+      <c r="Z27" s="142"/>
+      <c r="AA27" s="142"/>
+      <c r="AB27" s="142"/>
+      <c r="AC27" s="142"/>
+      <c r="AD27" s="143"/>
     </row>
     <row r="28" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="H28" s="163" t="s">
+      <c r="H28" s="106" t="s">
         <v>43</v>
       </c>
-      <c r="I28" s="164"/>
-      <c r="J28" s="165"/>
-      <c r="L28" s="179" t="s">
+      <c r="I28" s="107"/>
+      <c r="J28" s="108"/>
+      <c r="L28" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="M28" s="180"/>
-      <c r="N28" s="180"/>
-      <c r="O28" s="180"/>
-      <c r="P28" s="180"/>
-      <c r="Q28" s="181"/>
-      <c r="S28" s="174" t="s">
+      <c r="M28" s="126"/>
+      <c r="N28" s="126"/>
+      <c r="O28" s="126"/>
+      <c r="P28" s="126"/>
+      <c r="Q28" s="127"/>
+      <c r="S28" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="T28" s="175"/>
+      <c r="T28" s="120"/>
     </row>
     <row r="29" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="L29" s="182"/>
-      <c r="M29" s="183"/>
-      <c r="N29" s="183"/>
-      <c r="O29" s="183"/>
-      <c r="P29" s="183"/>
-      <c r="Q29" s="184"/>
-      <c r="W29" s="155" t="s">
+      <c r="L29" s="128"/>
+      <c r="M29" s="129"/>
+      <c r="N29" s="129"/>
+      <c r="O29" s="129"/>
+      <c r="P29" s="129"/>
+      <c r="Q29" s="130"/>
+      <c r="W29" s="144" t="s">
         <v>30</v>
       </c>
-      <c r="X29" s="156"/>
-      <c r="Y29" s="156"/>
-      <c r="Z29" s="156"/>
-      <c r="AA29" s="156"/>
-      <c r="AB29" s="156"/>
-      <c r="AC29" s="156"/>
-      <c r="AD29" s="157"/>
+      <c r="X29" s="145"/>
+      <c r="Y29" s="145"/>
+      <c r="Z29" s="145"/>
+      <c r="AA29" s="145"/>
+      <c r="AB29" s="145"/>
+      <c r="AC29" s="145"/>
+      <c r="AD29" s="146"/>
     </row>
     <row r="30" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="L30" s="160" t="s">
+      <c r="L30" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="M30" s="161"/>
-      <c r="N30" s="161"/>
-      <c r="O30" s="161"/>
-      <c r="P30" s="161"/>
-      <c r="Q30" s="162"/>
+      <c r="M30" s="104"/>
+      <c r="N30" s="104"/>
+      <c r="O30" s="104"/>
+      <c r="P30" s="104"/>
+      <c r="Q30" s="105"/>
       <c r="W30" s="4" t="s">
         <v>21</v>
       </c>
       <c r="X30" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="Y30" s="151" t="s">
+      <c r="Y30" s="140" t="s">
         <v>27</v>
       </c>
-      <c r="Z30" s="151"/>
-      <c r="AA30" s="151"/>
-      <c r="AB30" s="151"/>
-      <c r="AC30" s="151"/>
-      <c r="AD30" s="152"/>
+      <c r="Z30" s="140"/>
+      <c r="AA30" s="140"/>
+      <c r="AB30" s="140"/>
+      <c r="AC30" s="140"/>
+      <c r="AD30" s="141"/>
     </row>
     <row r="31" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="L31" s="163" t="s">
+      <c r="L31" s="106" t="s">
         <v>44</v>
       </c>
-      <c r="M31" s="164"/>
-      <c r="N31" s="164"/>
-      <c r="O31" s="164"/>
-      <c r="P31" s="164"/>
-      <c r="Q31" s="165"/>
+      <c r="M31" s="107"/>
+      <c r="N31" s="107"/>
+      <c r="O31" s="107"/>
+      <c r="P31" s="107"/>
+      <c r="Q31" s="108"/>
       <c r="W31" s="6" t="s">
         <v>25</v>
       </c>
       <c r="X31" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="Y31" s="151" t="s">
+      <c r="Y31" s="140" t="s">
         <v>26</v>
       </c>
-      <c r="Z31" s="151"/>
-      <c r="AA31" s="151"/>
-      <c r="AB31" s="151"/>
-      <c r="AC31" s="151"/>
-      <c r="AD31" s="152"/>
+      <c r="Z31" s="140"/>
+      <c r="AA31" s="140"/>
+      <c r="AB31" s="140"/>
+      <c r="AC31" s="140"/>
+      <c r="AD31" s="141"/>
     </row>
     <row r="32" spans="2:36" x14ac:dyDescent="0.25">
       <c r="W32" s="8" t="s">
@@ -3829,14 +3819,14 @@
       <c r="X32" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="Y32" s="151" t="s">
+      <c r="Y32" s="140" t="s">
         <v>28</v>
       </c>
-      <c r="Z32" s="151"/>
-      <c r="AA32" s="151"/>
-      <c r="AB32" s="151"/>
-      <c r="AC32" s="151"/>
-      <c r="AD32" s="152"/>
+      <c r="Z32" s="140"/>
+      <c r="AA32" s="140"/>
+      <c r="AB32" s="140"/>
+      <c r="AC32" s="140"/>
+      <c r="AD32" s="141"/>
     </row>
     <row r="33" spans="19:30" x14ac:dyDescent="0.25">
       <c r="S33" s="14"/>
@@ -3846,25 +3836,78 @@
       <c r="X33" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Y33" s="153" t="s">
+      <c r="Y33" s="142" t="s">
         <v>29</v>
       </c>
-      <c r="Z33" s="153"/>
-      <c r="AA33" s="153"/>
-      <c r="AB33" s="153"/>
-      <c r="AC33" s="153"/>
-      <c r="AD33" s="154"/>
+      <c r="Z33" s="142"/>
+      <c r="AA33" s="142"/>
+      <c r="AB33" s="142"/>
+      <c r="AC33" s="142"/>
+      <c r="AD33" s="143"/>
     </row>
   </sheetData>
   <mergeCells count="91">
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="I20:P20"/>
-    <mergeCell ref="I21:P21"/>
-    <mergeCell ref="V20:AC20"/>
-    <mergeCell ref="V21:AC21"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="AB10:AC10"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AG15:AG16"/>
+    <mergeCell ref="AD15:AF16"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="AD12:AJ13"/>
+    <mergeCell ref="AD9:AJ10"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="AH15:AJ16"/>
+    <mergeCell ref="AD5:AJ5"/>
+    <mergeCell ref="AD2:AJ3"/>
+    <mergeCell ref="I2:J3"/>
+    <mergeCell ref="AB2:AC3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="L25:Q25"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="H4:AD4"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="B2:H3"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="Y32:AD32"/>
+    <mergeCell ref="Y33:AD33"/>
+    <mergeCell ref="W23:AD23"/>
+    <mergeCell ref="Y24:AD24"/>
+    <mergeCell ref="Y25:AD25"/>
+    <mergeCell ref="Y26:AD26"/>
+    <mergeCell ref="Y27:AD27"/>
+    <mergeCell ref="W29:AD29"/>
+    <mergeCell ref="Y30:AD30"/>
+    <mergeCell ref="Y31:AD31"/>
     <mergeCell ref="L30:Q30"/>
     <mergeCell ref="L31:Q31"/>
     <mergeCell ref="H28:J28"/>
@@ -3881,73 +3924,20 @@
     <mergeCell ref="H25:J25"/>
     <mergeCell ref="H26:J26"/>
     <mergeCell ref="H27:J27"/>
-    <mergeCell ref="Y32:AD32"/>
-    <mergeCell ref="Y33:AD33"/>
-    <mergeCell ref="W23:AD23"/>
-    <mergeCell ref="Y24:AD24"/>
-    <mergeCell ref="Y25:AD25"/>
-    <mergeCell ref="Y26:AD26"/>
-    <mergeCell ref="Y27:AD27"/>
-    <mergeCell ref="W29:AD29"/>
-    <mergeCell ref="Y30:AD30"/>
-    <mergeCell ref="Y31:AD31"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="I20:P20"/>
+    <mergeCell ref="I21:P21"/>
+    <mergeCell ref="V20:AC20"/>
+    <mergeCell ref="V21:AC21"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="AB10:AC10"/>
     <mergeCell ref="AB8:AC8"/>
     <mergeCell ref="AB13:AC13"/>
     <mergeCell ref="AB11:AC11"/>
     <mergeCell ref="AB14:AC14"/>
     <mergeCell ref="AB9:AC9"/>
     <mergeCell ref="AB12:AC12"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L25:Q25"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="H4:AD4"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="B2:H3"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="AD5:AJ5"/>
-    <mergeCell ref="AD2:AJ3"/>
-    <mergeCell ref="I2:J3"/>
-    <mergeCell ref="AB2:AC3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="AD12:AJ13"/>
-    <mergeCell ref="AD9:AJ10"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AG15:AG16"/>
-    <mergeCell ref="AD15:AF16"/>
-    <mergeCell ref="AH15:AJ16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>